<commit_message>
Area and Density plots and data
</commit_message>
<xml_diff>
--- a/data/intermediate/dataset.xlsx
+++ b/data/intermediate/dataset.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Ariana</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>house_with_public_sanitation</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>density</t>
   </si>
 </sst>
 </file>
@@ -166,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,13 +183,30 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,8 +223,20 @@
         <fgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAECF0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -288,12 +323,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA2A9B1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFA2A9B1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA2A9B1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA2A9B1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFA2A9B1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA2A9B1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFA2A9B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
@@ -353,6 +416,18 @@
     <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -656,1802 +731,1953 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10">
-        <v>439378</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="B2" s="20">
+        <v>482</v>
+      </c>
+      <c r="C2" s="21">
+        <v>1195.2</v>
+      </c>
+      <c r="D2" s="19">
+        <v>576088</v>
+      </c>
+      <c r="E2" s="11">
         <v>151397</v>
       </c>
-      <c r="D2" s="12">
+      <c r="F2" s="12">
         <v>150444</v>
       </c>
-      <c r="E2" s="12">
+      <c r="G2" s="12">
         <v>794</v>
       </c>
-      <c r="F2" s="12">
+      <c r="H2" s="12">
         <v>134</v>
       </c>
-      <c r="G2" s="10">
+      <c r="I2" s="10">
         <v>180575</v>
       </c>
-      <c r="H2" s="13">
+      <c r="J2" s="13">
         <v>176993</v>
       </c>
-      <c r="I2" s="13">
+      <c r="K2" s="13">
         <v>99430</v>
       </c>
-      <c r="J2" s="13">
+      <c r="L2" s="13">
         <v>171553</v>
       </c>
-      <c r="K2" s="13">
+      <c r="M2" s="13">
         <v>154166</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>801</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>20926</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>26.124843945068701</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>18</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>21.158917027925199</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>3</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>63</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>60</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>3</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>63</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>60</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>447.699769794622</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="10">
-        <v>234922</v>
-      </c>
-      <c r="C3" s="11">
+      <c r="B3" s="19">
+        <v>3740</v>
+      </c>
+      <c r="C3" s="20">
+        <v>81.02</v>
+      </c>
+      <c r="D3" s="19">
+        <v>303032</v>
+      </c>
+      <c r="E3" s="11">
         <v>76827</v>
       </c>
-      <c r="D3" s="12">
+      <c r="F3" s="12">
         <v>60986</v>
       </c>
-      <c r="E3" s="12">
+      <c r="G3" s="12">
         <v>9742</v>
       </c>
-      <c r="F3" s="12">
+      <c r="H3" s="12">
         <v>915</v>
       </c>
-      <c r="G3" s="10">
+      <c r="I3" s="10">
         <v>85235</v>
       </c>
-      <c r="H3" s="13">
+      <c r="J3" s="13">
         <v>82178</v>
       </c>
-      <c r="I3" s="13">
+      <c r="K3" s="13">
         <v>0</v>
       </c>
-      <c r="J3" s="13">
+      <c r="L3" s="13">
         <v>64667</v>
       </c>
-      <c r="K3" s="13">
+      <c r="M3" s="13">
         <v>43223</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>5102</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>30347</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>5.9480595844766802</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>4</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>5.6593697919953296</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>3</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>61</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>58</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>34</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>4</v>
       </c>
-      <c r="V3">
+      <c r="X3">
         <v>57</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>32.028466442549302</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="14">
-        <v>484240</v>
-      </c>
-      <c r="C4" s="15">
+      <c r="B4" s="20">
+        <v>761</v>
+      </c>
+      <c r="C4" s="20">
+        <v>830.28</v>
+      </c>
+      <c r="D4" s="19">
+        <v>631842</v>
+      </c>
+      <c r="E4" s="15">
         <v>163811</v>
       </c>
-      <c r="D4" s="16">
+      <c r="F4" s="16">
         <v>162999</v>
       </c>
-      <c r="E4" s="16">
+      <c r="G4" s="16">
         <v>400</v>
       </c>
-      <c r="F4" s="16">
+      <c r="H4" s="16">
         <v>334</v>
       </c>
-      <c r="G4" s="14">
+      <c r="I4" s="14">
         <v>193050</v>
       </c>
-      <c r="H4" s="17">
+      <c r="J4" s="17">
         <v>188783</v>
       </c>
-      <c r="I4" s="17">
+      <c r="K4" s="17">
         <v>110192</v>
       </c>
-      <c r="J4" s="17">
+      <c r="L4" s="17">
         <v>183443</v>
       </c>
-      <c r="K4" s="17">
+      <c r="M4" s="17">
         <v>176411</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>1000</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>25576</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>25.576000000000001</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>16</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>21.4965630741289</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>4</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>63</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>59</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>35</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <v>63</v>
       </c>
-      <c r="V4">
+      <c r="X4">
         <v>59</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <v>462.10222400000299</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14">
-        <v>433289</v>
-      </c>
-      <c r="C5" s="15">
+      <c r="B5" s="19">
+        <v>3750</v>
+      </c>
+      <c r="C5" s="20">
+        <v>151.53</v>
+      </c>
+      <c r="D5" s="19">
+        <v>568219</v>
+      </c>
+      <c r="E5" s="15">
         <v>142532</v>
       </c>
-      <c r="D5" s="16">
+      <c r="F5" s="16">
         <v>126979</v>
       </c>
-      <c r="E5" s="16">
+      <c r="G5" s="16">
         <v>5575</v>
       </c>
-      <c r="F5" s="16">
+      <c r="H5" s="16">
         <v>3483</v>
       </c>
-      <c r="G5" s="14">
+      <c r="I5" s="14">
         <v>173508</v>
       </c>
-      <c r="H5" s="17">
+      <c r="J5" s="17">
         <v>165411</v>
       </c>
-      <c r="I5" s="17">
+      <c r="K5" s="17">
         <v>0</v>
       </c>
-      <c r="J5" s="17">
+      <c r="L5" s="17">
         <v>144994</v>
       </c>
-      <c r="K5" s="17">
+      <c r="M5" s="17">
         <v>122087</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>4925</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>35872</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>7.2836548223350297</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>4</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>9.2044431360242704</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>3</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>63</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>60</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>47</v>
       </c>
-      <c r="U5">
+      <c r="W5">
         <v>4</v>
       </c>
-      <c r="V5">
+      <c r="X5">
         <v>61</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>84.721773444304304</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="10">
-        <v>190564</v>
-      </c>
-      <c r="C6" s="11">
+      <c r="B6" s="19">
+        <v>4965</v>
+      </c>
+      <c r="C6" s="20">
+        <v>48.97</v>
+      </c>
+      <c r="D6" s="19">
+        <v>243156</v>
+      </c>
+      <c r="E6" s="11">
         <v>63708</v>
       </c>
-      <c r="D6" s="12">
+      <c r="F6" s="12">
         <v>48230</v>
       </c>
-      <c r="E6" s="12">
+      <c r="G6" s="12">
         <v>5875</v>
       </c>
-      <c r="F6" s="12">
+      <c r="H6" s="12">
         <v>4930</v>
       </c>
-      <c r="G6" s="10">
+      <c r="I6" s="10">
         <v>73632</v>
       </c>
-      <c r="H6" s="13">
+      <c r="J6" s="13">
         <v>70497</v>
       </c>
-      <c r="I6" s="13">
+      <c r="K6" s="13">
         <v>0</v>
       </c>
-      <c r="J6" s="13">
+      <c r="L6" s="13">
         <v>52461</v>
       </c>
-      <c r="K6" s="13">
+      <c r="M6" s="13">
         <v>39816</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>7253</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>36928</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>5.0914104508479197</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>4</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>4.5106671502373104</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>3</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>59</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>56</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>38</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <v>4</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <v>51</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <v>20.346118140230001</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="14">
-        <v>283098</v>
-      </c>
-      <c r="C7" s="15">
+      <c r="B7" s="19">
+        <v>7166</v>
+      </c>
+      <c r="C7" s="20">
+        <v>52.23</v>
+      </c>
+      <c r="D7" s="19">
+        <v>374300</v>
+      </c>
+      <c r="E7" s="15">
         <v>84783</v>
       </c>
-      <c r="D7" s="16">
+      <c r="F7" s="16">
         <v>81866</v>
       </c>
-      <c r="E7" s="16">
+      <c r="G7" s="16">
         <v>452</v>
       </c>
-      <c r="F7" s="16">
+      <c r="H7" s="16">
         <v>2368</v>
       </c>
-      <c r="G7" s="14">
+      <c r="I7" s="14">
         <v>107094</v>
       </c>
-      <c r="H7" s="17">
+      <c r="J7" s="17">
         <v>102115</v>
       </c>
-      <c r="I7" s="17">
+      <c r="K7" s="17">
         <v>4088</v>
       </c>
-      <c r="J7" s="17">
+      <c r="L7" s="17">
         <v>95050</v>
       </c>
-      <c r="K7" s="17">
+      <c r="M7" s="17">
         <v>64814</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>10466</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>59084</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>5.6453277278807601</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>4</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>7.6711596191908598</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>3</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>63</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>60</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>42</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <v>3</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>61</v>
       </c>
-      <c r="W7">
+      <c r="Y7">
         <v>58.846689903104398</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="10">
-        <v>255819</v>
-      </c>
-      <c r="C8" s="11">
+      <c r="B8" s="19">
+        <v>7807</v>
+      </c>
+      <c r="C8" s="20">
+        <v>43.21</v>
+      </c>
+      <c r="D8" s="19">
+        <v>337331</v>
+      </c>
+      <c r="E8" s="11">
         <v>77964</v>
       </c>
-      <c r="D8" s="12">
+      <c r="F8" s="12">
         <v>70705</v>
       </c>
-      <c r="E8" s="12">
+      <c r="G8" s="12">
         <v>3295</v>
       </c>
-      <c r="F8" s="12">
+      <c r="H8" s="12">
         <v>3590</v>
       </c>
-      <c r="G8" s="10">
+      <c r="I8" s="10">
         <v>89946</v>
       </c>
-      <c r="H8" s="13">
+      <c r="J8" s="13">
         <v>83747</v>
       </c>
-      <c r="I8" s="13">
+      <c r="K8" s="13">
         <v>0</v>
       </c>
-      <c r="J8" s="13">
+      <c r="L8" s="13">
         <v>72483</v>
       </c>
-      <c r="K8" s="13">
+      <c r="M8" s="13">
         <v>47280</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>10436</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>56002</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>5.36623227290149</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>4</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>6.2690587926838397</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>3</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>63</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>60</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>48</v>
       </c>
-      <c r="U8">
+      <c r="W8">
         <v>4</v>
       </c>
-      <c r="V8">
+      <c r="X8">
         <v>60</v>
       </c>
-      <c r="W8">
+      <c r="Y8">
         <v>39.301098146126499</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="14">
-        <v>311827</v>
-      </c>
-      <c r="C9" s="15">
+      <c r="B9" s="19">
+        <v>3102</v>
+      </c>
+      <c r="C9" s="20">
+        <v>129.43</v>
+      </c>
+      <c r="D9" s="19">
+        <v>401477</v>
+      </c>
+      <c r="E9" s="15">
         <v>103042</v>
       </c>
-      <c r="D9" s="16">
+      <c r="F9" s="16">
         <v>70589</v>
       </c>
-      <c r="E9" s="16">
+      <c r="G9" s="16">
         <v>8120</v>
       </c>
-      <c r="F9" s="16">
+      <c r="H9" s="16">
         <v>3918</v>
       </c>
-      <c r="G9" s="14">
+      <c r="I9" s="14">
         <v>122576</v>
       </c>
-      <c r="H9" s="17">
+      <c r="J9" s="17">
         <v>118554</v>
       </c>
-      <c r="I9" s="17">
+      <c r="K9" s="17">
         <v>0</v>
       </c>
-      <c r="J9" s="17">
+      <c r="L9" s="17">
         <v>76912</v>
       </c>
-      <c r="K9" s="17">
+      <c r="M9" s="17">
         <v>43871</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>4431</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>28223</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>6.36944256375536</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>5</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>5.5927021176314202</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>3</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>56</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>53</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>30</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <v>4</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>51</v>
       </c>
-      <c r="W9">
+      <c r="Y9">
         <v>31.278316976558902</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="10">
-        <v>414094</v>
-      </c>
-      <c r="C10" s="11">
+      <c r="B10" s="19">
+        <v>6712</v>
+      </c>
+      <c r="C10" s="20">
+        <v>85.01</v>
+      </c>
+      <c r="D10" s="19">
+        <v>570559</v>
+      </c>
+      <c r="E10" s="11">
         <v>129902</v>
       </c>
-      <c r="D10" s="12">
+      <c r="F10" s="12">
         <v>90573</v>
       </c>
-      <c r="E10" s="12">
+      <c r="G10" s="12">
         <v>24463</v>
       </c>
-      <c r="F10" s="12">
+      <c r="H10" s="12">
         <v>14091</v>
       </c>
-      <c r="G10" s="10">
+      <c r="I10" s="10">
         <v>154586</v>
       </c>
-      <c r="H10" s="13">
+      <c r="J10" s="13">
         <v>143229</v>
       </c>
-      <c r="I10" s="13">
+      <c r="K10" s="13">
         <v>2238</v>
       </c>
-      <c r="J10" s="13">
+      <c r="L10" s="13">
         <v>98059</v>
       </c>
-      <c r="K10" s="13">
+      <c r="M10" s="13">
         <v>49463</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>9483</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>63185</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>6.6629758515237798</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>5</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>5.78713834669162</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>3</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>63</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>60</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>46</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <v>4</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <v>60</v>
       </c>
-      <c r="W10">
+      <c r="Y10">
         <v>33.490970243748599</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="14">
-        <v>318062</v>
-      </c>
-      <c r="C11" s="15">
+      <c r="B11" s="19">
+        <v>8260</v>
+      </c>
+      <c r="C11" s="20">
+        <v>53.18</v>
+      </c>
+      <c r="D11" s="19">
+        <v>439243</v>
+      </c>
+      <c r="E11" s="15">
         <v>95292</v>
       </c>
-      <c r="D11" s="16">
+      <c r="F11" s="16">
         <v>62733</v>
       </c>
-      <c r="E11" s="16">
+      <c r="G11" s="16">
         <v>7939</v>
       </c>
-      <c r="F11" s="16">
+      <c r="H11" s="16">
         <v>22529</v>
       </c>
-      <c r="G11" s="14">
+      <c r="I11" s="14">
         <v>105980</v>
       </c>
-      <c r="H11" s="17">
+      <c r="J11" s="17">
         <v>98460</v>
       </c>
-      <c r="I11" s="17">
+      <c r="K11" s="17">
         <v>4557</v>
       </c>
-      <c r="J11" s="17">
+      <c r="L11" s="17">
         <v>63787</v>
       </c>
-      <c r="K11" s="17">
+      <c r="M11" s="17">
         <v>34973</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>11479</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>62082</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>5.4083108284693804</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>4</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>5.1966574320904302</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>2</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>62</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>60</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <v>2</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <v>4</v>
       </c>
-      <c r="V11">
+      <c r="X11">
         <v>60</v>
       </c>
-      <c r="W11">
+      <c r="Y11">
         <v>27.005248466500699</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="10">
-        <v>118261</v>
-      </c>
-      <c r="C12" s="11">
+      <c r="B12" s="19">
+        <v>22454</v>
+      </c>
+      <c r="C12" s="20">
+        <v>6.99</v>
+      </c>
+      <c r="D12" s="19">
+        <v>156961</v>
+      </c>
+      <c r="E12" s="11">
         <v>34285</v>
       </c>
-      <c r="D12" s="12">
+      <c r="F12" s="12">
         <v>33979</v>
       </c>
-      <c r="E12" s="12">
+      <c r="G12" s="12">
         <v>222</v>
       </c>
-      <c r="F12" s="12">
+      <c r="H12" s="12">
         <v>56</v>
       </c>
-      <c r="G12" s="10">
+      <c r="I12" s="10">
         <v>40395</v>
       </c>
-      <c r="H12" s="13">
+      <c r="J12" s="13">
         <v>37323</v>
       </c>
-      <c r="I12" s="13">
+      <c r="K12" s="13">
         <v>0</v>
       </c>
-      <c r="J12" s="13">
+      <c r="L12" s="13">
         <v>36190</v>
       </c>
-      <c r="K12" s="13">
+      <c r="M12" s="13">
         <v>13935</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>30508</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>121444</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>3.98072636685459</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>3</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>3.5774809350742398</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>2</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>63</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>61</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>44</v>
       </c>
-      <c r="U12">
+      <c r="W12">
         <v>3</v>
       </c>
-      <c r="V12">
+      <c r="X12">
         <v>61</v>
       </c>
-      <c r="W12">
+      <c r="Y12">
         <v>12.7983698408196</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="10">
-        <v>297933</v>
-      </c>
-      <c r="C13" s="11">
+      <c r="B13" s="19">
+        <v>2966</v>
+      </c>
+      <c r="C13" s="20">
+        <v>138.51</v>
+      </c>
+      <c r="D13" s="19">
+        <v>410812</v>
+      </c>
+      <c r="E13" s="11">
         <v>95466</v>
       </c>
-      <c r="D13" s="12">
+      <c r="F13" s="12">
         <v>86178</v>
       </c>
-      <c r="E13" s="12">
+      <c r="G13" s="12">
         <v>16</v>
       </c>
-      <c r="F13" s="12">
+      <c r="H13" s="12">
         <v>16</v>
       </c>
-      <c r="G13" s="10">
+      <c r="I13" s="10">
         <v>124958</v>
       </c>
-      <c r="H13" s="13">
+      <c r="J13" s="13">
         <v>120528</v>
       </c>
-      <c r="I13" s="13">
+      <c r="K13" s="13">
         <v>12684</v>
       </c>
-      <c r="J13" s="13">
+      <c r="L13" s="13">
         <v>112526</v>
       </c>
-      <c r="K13" s="13">
+      <c r="M13" s="13">
         <v>48445</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>4193</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>42885</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>10.227760553303099</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>7</v>
       </c>
-      <c r="P13">
+      <c r="R13">
         <v>8.4307689550412608</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>3</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>63</v>
       </c>
-      <c r="S13">
+      <c r="U13">
         <v>60</v>
       </c>
-      <c r="T13">
+      <c r="V13">
         <v>54</v>
       </c>
-      <c r="U13">
+      <c r="W13">
         <v>6</v>
       </c>
-      <c r="V13">
+      <c r="X13">
         <v>61</v>
       </c>
-      <c r="W13">
+      <c r="Y13">
         <v>71.077865173287506</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="10">
-        <v>292810</v>
-      </c>
-      <c r="C14" s="11">
+      <c r="B14" s="19">
+        <v>1137</v>
+      </c>
+      <c r="C14" s="20">
+        <v>333.79</v>
+      </c>
+      <c r="D14" s="19">
+        <v>379518</v>
+      </c>
+      <c r="E14" s="11">
         <v>95405</v>
       </c>
-      <c r="D14" s="12">
+      <c r="F14" s="12">
         <v>93757</v>
       </c>
-      <c r="E14" s="12">
+      <c r="G14" s="12">
         <v>1043</v>
       </c>
-      <c r="F14" s="12">
+      <c r="H14" s="12">
         <v>245</v>
       </c>
-      <c r="G14" s="10">
+      <c r="I14" s="10">
         <v>103254</v>
       </c>
-      <c r="H14" s="13">
+      <c r="J14" s="13">
         <v>100900</v>
       </c>
-      <c r="I14" s="13">
+      <c r="K14" s="13">
         <v>41639</v>
       </c>
-      <c r="J14" s="13">
+      <c r="L14" s="13">
         <v>96614</v>
       </c>
-      <c r="K14" s="13">
+      <c r="M14" s="13">
         <v>80342</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>1473</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>18115</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>12.298031228784801</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>7</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>11.4609690457124</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>3</v>
       </c>
-      <c r="R14">
+      <c r="T14">
         <v>63</v>
       </c>
-      <c r="S14">
+      <c r="U14">
         <v>60</v>
       </c>
-      <c r="T14">
+      <c r="V14">
         <v>50</v>
       </c>
-      <c r="U14">
+      <c r="W14">
         <v>4</v>
       </c>
-      <c r="V14">
+      <c r="X14">
         <v>60</v>
       </c>
-      <c r="W14">
+      <c r="Y14">
         <v>131.35381146677699</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="10">
-        <v>358126</v>
-      </c>
-      <c r="C15" s="11">
+      <c r="B15" s="19">
+        <v>9167</v>
+      </c>
+      <c r="C15" s="20">
+        <v>52.31</v>
+      </c>
+      <c r="D15" s="19">
+        <v>479520</v>
+      </c>
+      <c r="E15" s="11">
         <v>113277</v>
       </c>
-      <c r="D15" s="12">
+      <c r="F15" s="12">
         <v>104976</v>
       </c>
-      <c r="E15" s="12">
+      <c r="G15" s="12">
         <v>1401</v>
       </c>
-      <c r="F15" s="12">
+      <c r="H15" s="12">
         <v>6899</v>
       </c>
-      <c r="G15" s="10">
+      <c r="I15" s="10">
         <v>164871</v>
       </c>
-      <c r="H15" s="13">
+      <c r="J15" s="13">
         <v>156819</v>
       </c>
-      <c r="I15" s="13">
+      <c r="K15" s="13">
         <v>0</v>
       </c>
-      <c r="J15" s="13">
+      <c r="L15" s="13">
         <v>142497</v>
       </c>
-      <c r="K15" s="13">
+      <c r="M15" s="13">
         <v>31771</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>12040</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>81413</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>6.7618770764119596</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>4</v>
       </c>
-      <c r="P15">
+      <c r="R15">
         <v>9.2521358833240992</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>3</v>
       </c>
-      <c r="R15">
+      <c r="T15">
         <v>63</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>60</v>
       </c>
-      <c r="T15">
+      <c r="V15">
         <v>58</v>
       </c>
-      <c r="U15">
+      <c r="W15">
         <v>4</v>
       </c>
-      <c r="V15">
+      <c r="X15">
         <v>61</v>
       </c>
-      <c r="W15">
+      <c r="Y15">
         <v>85.602018403493304</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="14">
-        <v>403251</v>
-      </c>
-      <c r="C16" s="15">
+      <c r="B16" s="19">
+        <v>1019</v>
+      </c>
+      <c r="C16" s="20">
+        <v>538.59</v>
+      </c>
+      <c r="D16" s="19">
+        <v>548828</v>
+      </c>
+      <c r="E16" s="15">
         <v>133595</v>
       </c>
-      <c r="D16" s="16">
+      <c r="F16" s="16">
         <v>133256</v>
       </c>
-      <c r="E16" s="16">
+      <c r="G16" s="16">
         <v>74</v>
       </c>
-      <c r="F16" s="16">
+      <c r="H16" s="16">
         <v>257</v>
       </c>
-      <c r="G16" s="14">
+      <c r="I16" s="14">
         <v>164687</v>
       </c>
-      <c r="H16" s="17">
+      <c r="J16" s="17">
         <v>161095</v>
       </c>
-      <c r="I16" s="17">
+      <c r="K16" s="17">
         <v>38987</v>
       </c>
-      <c r="J16" s="17">
+      <c r="L16" s="17">
         <v>156267</v>
       </c>
-      <c r="K16" s="17">
+      <c r="M16" s="17">
         <v>137155</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>1414</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>34291</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>24.251060820367801</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>17</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <v>18.310226878750601</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>3</v>
       </c>
-      <c r="R16">
+      <c r="T16">
         <v>63</v>
       </c>
-      <c r="S16">
+      <c r="U16">
         <v>60</v>
       </c>
-      <c r="T16">
+      <c r="V16">
         <v>3</v>
       </c>
-      <c r="U16">
+      <c r="W16">
         <v>6</v>
       </c>
-      <c r="V16">
+      <c r="X16">
         <v>61</v>
       </c>
-      <c r="W16">
+      <c r="Y16">
         <v>335.264408351322</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="14">
-        <v>596412</v>
-      </c>
-      <c r="C17" s="15">
+      <c r="B17" s="19">
+        <v>2788</v>
+      </c>
+      <c r="C17" s="20">
+        <v>282.61</v>
+      </c>
+      <c r="D17" s="19">
+        <v>787920</v>
+      </c>
+      <c r="E17" s="15">
         <v>202554</v>
       </c>
-      <c r="D17" s="16">
+      <c r="F17" s="16">
         <v>180130</v>
       </c>
-      <c r="E17" s="16">
+      <c r="G17" s="16">
         <v>9979</v>
       </c>
-      <c r="F17" s="16">
+      <c r="H17" s="16">
         <v>12029</v>
       </c>
-      <c r="G17" s="14">
+      <c r="I17" s="14">
         <v>257580</v>
       </c>
-      <c r="H17" s="17">
+      <c r="J17" s="17">
         <v>252914</v>
       </c>
-      <c r="I17" s="17">
+      <c r="K17" s="17">
         <v>90459</v>
       </c>
-      <c r="J17" s="17">
+      <c r="L17" s="17">
         <v>227978</v>
       </c>
-      <c r="K17" s="17">
+      <c r="M17" s="17">
         <v>176272</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>4139</v>
       </c>
-      <c r="M17">
+      <c r="O17">
         <v>60223</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <v>14.5501328823387</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>8</v>
       </c>
-      <c r="P17">
+      <c r="R17">
         <v>14.3608144072325</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>3</v>
       </c>
-      <c r="R17">
+      <c r="T17">
         <v>63</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>60</v>
       </c>
-      <c r="T17">
+      <c r="V17">
         <v>46</v>
       </c>
-      <c r="U17">
+      <c r="W17">
         <v>7</v>
       </c>
-      <c r="V17">
+      <c r="X17">
         <v>61</v>
       </c>
-      <c r="W17">
+      <c r="Y17">
         <v>206.23299043897501</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="14">
-        <v>724678</v>
-      </c>
-      <c r="C18" s="15">
+      <c r="B18" s="19">
+        <v>7545</v>
+      </c>
+      <c r="C18" s="20">
+        <v>126.63</v>
+      </c>
+      <c r="D18" s="19">
+        <v>1113496</v>
+      </c>
+      <c r="E18" s="15">
         <v>242740</v>
       </c>
-      <c r="D18" s="16">
+      <c r="F18" s="16">
         <v>219122</v>
       </c>
-      <c r="E18" s="16">
+      <c r="G18" s="16">
         <v>3701</v>
       </c>
-      <c r="F18" s="16">
+      <c r="H18" s="16">
         <v>19901</v>
       </c>
-      <c r="G18" s="14">
+      <c r="I18" s="14">
         <v>290872</v>
       </c>
-      <c r="H18" s="17">
+      <c r="J18" s="17">
         <v>284940</v>
       </c>
-      <c r="I18" s="17">
+      <c r="K18" s="17">
         <v>24043</v>
       </c>
-      <c r="J18" s="17">
+      <c r="L18" s="17">
         <v>251306</v>
       </c>
-      <c r="K18" s="17">
+      <c r="M18" s="17">
         <v>141098</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>10242</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>90720</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <v>8.8576449912126503</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>5</v>
       </c>
-      <c r="P18">
+      <c r="R18">
         <v>11.5116509008616</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <v>3</v>
       </c>
-      <c r="R18">
+      <c r="T18">
         <v>63</v>
       </c>
-      <c r="S18">
+      <c r="U18">
         <v>60</v>
       </c>
-      <c r="T18">
+      <c r="V18">
         <v>37</v>
       </c>
-      <c r="U18">
+      <c r="W18">
         <v>4</v>
       </c>
-      <c r="V18">
+      <c r="X18">
         <v>61</v>
       </c>
-      <c r="W18">
+      <c r="Y18">
         <v>132.51810646330901</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="10">
-        <v>319933</v>
-      </c>
-      <c r="C19" s="11">
+      <c r="B19" s="19">
+        <v>7405</v>
+      </c>
+      <c r="C19" s="20">
+        <v>58.06</v>
+      </c>
+      <c r="D19" s="19">
+        <v>429912</v>
+      </c>
+      <c r="E19" s="11">
         <v>93552</v>
       </c>
-      <c r="D19" s="12">
+      <c r="F19" s="12">
         <v>51822</v>
       </c>
-      <c r="E19" s="12">
+      <c r="G19" s="12">
         <v>12745</v>
       </c>
-      <c r="F19" s="12">
+      <c r="H19" s="12">
         <v>28775</v>
       </c>
-      <c r="G19" s="10">
+      <c r="I19" s="10">
         <v>110372</v>
       </c>
-      <c r="H19" s="13">
+      <c r="J19" s="13">
         <v>102603</v>
       </c>
-      <c r="I19" s="13">
+      <c r="K19" s="13">
         <v>0</v>
       </c>
-      <c r="J19" s="13">
+      <c r="L19" s="13">
         <v>56295</v>
       </c>
-      <c r="K19" s="13">
+      <c r="M19" s="13">
         <v>17558</v>
       </c>
-      <c r="L19">
+      <c r="N19">
         <v>10485</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <v>61777</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <v>5.8919408679065297</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>5</v>
       </c>
-      <c r="P19">
+      <c r="R19">
         <v>4.6521803463073104</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <v>3</v>
       </c>
-      <c r="R19">
+      <c r="T19">
         <v>63</v>
       </c>
-      <c r="S19">
+      <c r="U19">
         <v>60</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>41</v>
       </c>
-      <c r="U19">
+      <c r="W19">
         <v>4</v>
       </c>
-      <c r="V19">
+      <c r="X19">
         <v>59</v>
       </c>
-      <c r="W19">
+      <c r="Y19">
         <v>21.642781974567999</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="14">
-        <v>167706</v>
-      </c>
-      <c r="C20" s="15">
+      <c r="B20" s="19">
+        <v>4642</v>
+      </c>
+      <c r="C20" s="20">
+        <v>48.06</v>
+      </c>
+      <c r="D20" s="19">
+        <v>223087</v>
+      </c>
+      <c r="E20" s="15">
         <v>55028</v>
       </c>
-      <c r="D20" s="16">
+      <c r="F20" s="16">
         <v>40846</v>
       </c>
-      <c r="E20" s="16">
+      <c r="G20" s="16">
         <v>6699</v>
       </c>
-      <c r="F20" s="16">
+      <c r="H20" s="16">
         <v>2030</v>
       </c>
-      <c r="G20" s="14">
+      <c r="I20" s="14">
         <v>60471</v>
       </c>
-      <c r="H20" s="17">
+      <c r="J20" s="17">
         <v>55988</v>
       </c>
-      <c r="I20" s="17">
+      <c r="K20" s="17">
         <v>0</v>
       </c>
-      <c r="J20" s="17">
+      <c r="L20" s="17">
         <v>39689</v>
       </c>
-      <c r="K20" s="17">
+      <c r="M20" s="17">
         <v>28764</v>
       </c>
-      <c r="L20">
+      <c r="N20">
         <v>6763</v>
       </c>
-      <c r="M20">
+      <c r="O20">
         <v>32910</v>
       </c>
-      <c r="N20">
+      <c r="P20">
         <v>4.8661836463108097</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <v>4</v>
       </c>
-      <c r="P20">
+      <c r="R20">
         <v>3.8731913390491601</v>
       </c>
-      <c r="Q20">
+      <c r="S20">
         <v>3</v>
       </c>
-      <c r="R20">
+      <c r="T20">
         <v>53</v>
       </c>
-      <c r="S20">
+      <c r="U20">
         <v>50</v>
       </c>
-      <c r="T20">
+      <c r="V20">
         <v>43</v>
       </c>
-      <c r="U20">
+      <c r="W20">
         <v>4</v>
       </c>
-      <c r="V20">
+      <c r="X20">
         <v>44</v>
       </c>
-      <c r="W20">
+      <c r="Y20">
         <v>15.0016111488854</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="10">
-        <v>505579</v>
-      </c>
-      <c r="C21" s="11">
+      <c r="B21" s="19">
+        <v>2669</v>
+      </c>
+      <c r="C21" s="20">
+        <v>252.89</v>
+      </c>
+      <c r="D21" s="19">
+        <v>674971</v>
+      </c>
+      <c r="E21" s="11">
         <v>171114</v>
       </c>
-      <c r="D21" s="12">
+      <c r="F21" s="12">
         <v>169445</v>
       </c>
-      <c r="E21" s="12">
+      <c r="G21" s="12">
         <v>993</v>
       </c>
-      <c r="F21" s="12">
+      <c r="H21" s="12">
         <v>654</v>
       </c>
-      <c r="G21" s="10">
+      <c r="I21" s="10">
         <v>219373</v>
       </c>
-      <c r="H21" s="13">
+      <c r="J21" s="13">
         <v>215086</v>
       </c>
-      <c r="I21" s="13">
+      <c r="K21" s="13">
         <v>93390</v>
       </c>
-      <c r="J21" s="13">
+      <c r="L21" s="13">
         <v>207046</v>
       </c>
-      <c r="K21" s="13">
+      <c r="M21" s="13">
         <v>175437</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>3850</v>
       </c>
-      <c r="M21">
+      <c r="O21">
         <v>50456</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <v>13.105454545454499</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>7</v>
       </c>
-      <c r="P21">
+      <c r="R21">
         <v>15.0327191676227</v>
       </c>
-      <c r="Q21">
+      <c r="S21">
         <v>3</v>
       </c>
-      <c r="R21">
+      <c r="T21">
         <v>63</v>
       </c>
-      <c r="S21">
+      <c r="U21">
         <v>60</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <v>48</v>
       </c>
-      <c r="U21">
+      <c r="W21">
         <v>4</v>
       </c>
-      <c r="V21">
+      <c r="X21">
         <v>61</v>
       </c>
-      <c r="W21">
+      <c r="Y21">
         <v>225.98264557261101</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="14">
-        <v>112146</v>
-      </c>
-      <c r="C22" s="15">
+      <c r="B22" s="19">
+        <v>38889</v>
+      </c>
+      <c r="C22" s="20">
+        <v>3.84</v>
+      </c>
+      <c r="D22" s="19">
+        <v>149453</v>
+      </c>
+      <c r="E22" s="15">
         <v>30887</v>
       </c>
-      <c r="D22" s="16">
+      <c r="F22" s="16">
         <v>29166</v>
       </c>
-      <c r="E22" s="16">
+      <c r="G22" s="16">
         <v>160</v>
       </c>
-      <c r="F22" s="16">
+      <c r="H22" s="16">
         <v>1557</v>
       </c>
-      <c r="G22" s="14">
+      <c r="I22" s="14">
         <v>45492</v>
       </c>
-      <c r="H22" s="17">
+      <c r="J22" s="17">
         <v>42872</v>
       </c>
-      <c r="I22" s="17">
+      <c r="K22" s="17">
         <v>0</v>
       </c>
-      <c r="J22" s="17">
+      <c r="L22" s="17">
         <v>39590</v>
       </c>
-      <c r="K22" s="17">
+      <c r="M22" s="17">
         <v>18196</v>
       </c>
-      <c r="L22">
+      <c r="N22">
         <v>54331</v>
       </c>
-      <c r="M22">
+      <c r="O22">
         <v>224193</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <v>4.1264287423386303</v>
       </c>
-      <c r="O22">
+      <c r="Q22">
         <v>4</v>
       </c>
-      <c r="P22">
+      <c r="R22">
         <v>3.7606720792507602</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <v>2</v>
       </c>
-      <c r="R22">
+      <c r="T22">
         <v>62</v>
       </c>
-      <c r="S22">
+      <c r="U22">
         <v>60</v>
       </c>
-      <c r="T22">
+      <c r="V22">
         <v>2</v>
       </c>
-      <c r="U22">
+      <c r="W22">
         <v>3</v>
       </c>
-      <c r="V22">
+      <c r="X22">
         <v>61</v>
       </c>
-      <c r="W22">
+      <c r="Y22">
         <v>14.1426544876562</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="14">
-        <v>80157</v>
-      </c>
-      <c r="C23" s="15">
+      <c r="B23" s="19">
+        <v>5593</v>
+      </c>
+      <c r="C23" s="20">
+        <v>22.87</v>
+      </c>
+      <c r="D23" s="19">
+        <v>107912</v>
+      </c>
+      <c r="E23" s="15">
         <v>25566</v>
       </c>
-      <c r="D23" s="16">
+      <c r="F23" s="16">
         <v>25251</v>
       </c>
-      <c r="E23" s="16">
+      <c r="G23" s="16">
         <v>210</v>
       </c>
-      <c r="F23" s="16">
+      <c r="H23" s="16">
         <v>26</v>
       </c>
-      <c r="G23" s="14">
+      <c r="I23" s="14">
         <v>29683</v>
       </c>
-      <c r="H23" s="17">
+      <c r="J23" s="17">
         <v>27750</v>
       </c>
-      <c r="I23" s="17">
+      <c r="K23" s="17">
         <v>0</v>
       </c>
-      <c r="J23" s="17">
+      <c r="L23" s="17">
         <v>26873</v>
       </c>
-      <c r="K23" s="17">
+      <c r="M23" s="17">
         <v>20054</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>8630</v>
       </c>
-      <c r="M23">
+      <c r="O23">
         <v>38348</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <v>4.4435689455388196</v>
       </c>
-      <c r="O23">
+      <c r="Q23">
         <v>3</v>
       </c>
-      <c r="P23">
+      <c r="R23">
         <v>5.1634469124928</v>
       </c>
-      <c r="Q23">
+      <c r="S23">
         <v>2</v>
       </c>
-      <c r="R23">
+      <c r="T23">
         <v>63</v>
       </c>
-      <c r="S23">
+      <c r="U23">
         <v>61</v>
       </c>
-      <c r="T23">
+      <c r="V23">
         <v>48</v>
       </c>
-      <c r="U23">
+      <c r="W23">
         <v>3</v>
       </c>
-      <c r="V23">
+      <c r="X23">
         <v>61</v>
       </c>
-      <c r="W23">
+      <c r="Y23">
         <v>26.661184018131401</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="14">
-        <v>837597</v>
-      </c>
-      <c r="C24" s="15">
+      <c r="B24" s="20">
+        <v>288</v>
+      </c>
+      <c r="C24" s="21">
+        <v>3052.74</v>
+      </c>
+      <c r="D24" s="19">
+        <v>1056247</v>
+      </c>
+      <c r="E24" s="15">
         <v>287412</v>
       </c>
-      <c r="D24" s="16">
+      <c r="F24" s="16">
         <v>287006</v>
       </c>
-      <c r="E24" s="16">
+      <c r="G24" s="16">
         <v>219</v>
       </c>
-      <c r="F24" s="16">
+      <c r="H24" s="16">
         <v>169</v>
       </c>
-      <c r="G24" s="14">
+      <c r="I24" s="14">
         <v>343348</v>
       </c>
-      <c r="H24" s="17">
+      <c r="J24" s="17">
         <v>341456</v>
       </c>
-      <c r="I24" s="17">
+      <c r="K24" s="17">
         <v>205886</v>
       </c>
-      <c r="J24" s="17">
+      <c r="L24" s="17">
         <v>330896</v>
       </c>
-      <c r="K24" s="17">
+      <c r="M24" s="17">
         <v>333580</v>
       </c>
-      <c r="L24">
+      <c r="N24">
         <v>389</v>
       </c>
-      <c r="M24">
+      <c r="O24">
         <v>21723</v>
       </c>
-      <c r="N24">
+      <c r="P24">
         <v>55.843187660668399</v>
       </c>
-      <c r="O24">
+      <c r="Q24">
         <v>63</v>
       </c>
-      <c r="P24">
+      <c r="R24">
         <v>13.0635616821522</v>
       </c>
-      <c r="Q24">
+      <c r="S24">
         <v>11</v>
       </c>
-      <c r="R24">
+      <c r="T24">
         <v>63</v>
       </c>
-      <c r="S24">
+      <c r="U24">
         <v>52</v>
       </c>
-      <c r="T24">
+      <c r="V24">
         <v>13</v>
       </c>
-      <c r="U24">
+      <c r="W24">
         <v>63</v>
       </c>
-      <c r="V24">
+      <c r="X24">
         <v>48</v>
       </c>
-      <c r="W24">
+      <c r="Y24">
         <v>170.65664382339401</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="10">
-        <v>132349</v>
-      </c>
-      <c r="C25" s="11">
+      <c r="B25" s="19">
+        <v>2820</v>
+      </c>
+      <c r="C25" s="20">
+        <v>63.93</v>
+      </c>
+      <c r="D25" s="19">
+        <v>176945</v>
+      </c>
+      <c r="E25" s="11">
         <v>42835</v>
       </c>
-      <c r="D25" s="12">
+      <c r="F25" s="12">
         <v>34852</v>
       </c>
-      <c r="E25" s="12">
+      <c r="G25" s="12">
         <v>5625</v>
       </c>
-      <c r="F25" s="12">
+      <c r="H25" s="12">
         <v>1444</v>
       </c>
-      <c r="G25" s="10">
+      <c r="I25" s="10">
         <v>48363</v>
       </c>
-      <c r="H25" s="13">
+      <c r="J25" s="13">
         <v>46269</v>
       </c>
-      <c r="I25" s="13">
+      <c r="K25" s="13">
         <v>2981</v>
       </c>
-      <c r="J25" s="13">
+      <c r="L25" s="13">
         <v>36459</v>
       </c>
-      <c r="K25" s="13">
+      <c r="M25" s="13">
         <v>23622</v>
       </c>
-      <c r="L25">
+      <c r="N25">
         <v>4130</v>
       </c>
-      <c r="M25">
+      <c r="O25">
         <v>27330</v>
       </c>
-      <c r="N25">
+      <c r="P25">
         <v>6.61743341404358</v>
       </c>
-      <c r="O25">
+      <c r="Q25">
         <v>5</v>
       </c>
-      <c r="P25">
+      <c r="R25">
         <v>6.3587568034766102</v>
       </c>
-      <c r="Q25">
+      <c r="S25">
         <v>3</v>
       </c>
-      <c r="R25">
+      <c r="T25">
         <v>59</v>
       </c>
-      <c r="S25">
+      <c r="U25">
         <v>56</v>
       </c>
-      <c r="T25">
+      <c r="V25">
         <v>40</v>
       </c>
-      <c r="U25">
+      <c r="W25">
         <v>4</v>
       </c>
-      <c r="V25">
+      <c r="X25">
         <v>54</v>
       </c>
-      <c r="W25">
+      <c r="Y25">
         <v>40.433788085760099</v>
       </c>
     </row>

</xml_diff>